<commit_message>
Implement error handling and file logging for input data process
</commit_message>
<xml_diff>
--- a/FinalReport.xlsx
+++ b/FinalReport.xlsx
@@ -40,7 +40,7 @@
     <x:t>Success</x:t>
   </x:si>
   <x:si>
-    <x:t>1900043370</x:t>
+    <x:t>1900085467</x:t>
   </x:si>
   <x:si>
     <x:t>Successfully posted to Mock.</x:t>
@@ -52,7 +52,7 @@
     <x:t>PO-7891</x:t>
   </x:si>
   <x:si>
-    <x:t>1900051605</x:t>
+    <x:t>1900086618</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-003</x:t>
@@ -61,7 +61,7 @@
     <x:t>PO-7892</x:t>
   </x:si>
   <x:si>
-    <x:t>1900030509</x:t>
+    <x:t>1900028044</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-004</x:t>
@@ -70,7 +70,7 @@
     <x:t>PO-7893</x:t>
   </x:si>
   <x:si>
-    <x:t>1900035616</x:t>
+    <x:t>1900054503</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-005</x:t>
@@ -79,7 +79,7 @@
     <x:t>PO-7894</x:t>
   </x:si>
   <x:si>
-    <x:t>1900054352</x:t>
+    <x:t>1900054909</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-006</x:t>
@@ -88,7 +88,7 @@
     <x:t>PO-7895</x:t>
   </x:si>
   <x:si>
-    <x:t>1900076447</x:t>
+    <x:t>1900028623</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-008</x:t>
@@ -97,7 +97,7 @@
     <x:t>PO-7896</x:t>
   </x:si>
   <x:si>
-    <x:t>1900018390</x:t>
+    <x:t>1900010332</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-009</x:t>
@@ -106,7 +106,7 @@
     <x:t>PO-7897</x:t>
   </x:si>
   <x:si>
-    <x:t>1900041582</x:t>
+    <x:t>1900065727</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-010</x:t>
@@ -115,7 +115,7 @@
     <x:t>PO-7898</x:t>
   </x:si>
   <x:si>
-    <x:t>1900091327</x:t>
+    <x:t>1900030682</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -500,7 +500,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
         <x:v>9</x:v>
@@ -517,7 +517,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
         <x:v>9</x:v>
@@ -534,7 +534,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
         <x:v>9</x:v>
@@ -551,7 +551,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
         <x:v>9</x:v>
@@ -568,7 +568,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
         <x:v>9</x:v>
@@ -585,7 +585,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
         <x:v>9</x:v>
@@ -602,7 +602,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
         <x:v>9</x:v>
@@ -619,7 +619,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
         <x:v>9</x:v>
@@ -636,7 +636,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
         <x:v>9</x:v>

</xml_diff>

<commit_message>
Create main workflow to run all process steps
</commit_message>
<xml_diff>
--- a/FinalReport.xlsx
+++ b/FinalReport.xlsx
@@ -40,7 +40,7 @@
     <x:t>Success</x:t>
   </x:si>
   <x:si>
-    <x:t>1900085467</x:t>
+    <x:t>1900030872</x:t>
   </x:si>
   <x:si>
     <x:t>Successfully posted to Mock.</x:t>
@@ -52,7 +52,7 @@
     <x:t>PO-7891</x:t>
   </x:si>
   <x:si>
-    <x:t>1900086618</x:t>
+    <x:t>1900016668</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-003</x:t>
@@ -61,7 +61,7 @@
     <x:t>PO-7892</x:t>
   </x:si>
   <x:si>
-    <x:t>1900028044</x:t>
+    <x:t>1900036977</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-004</x:t>
@@ -70,7 +70,7 @@
     <x:t>PO-7893</x:t>
   </x:si>
   <x:si>
-    <x:t>1900054503</x:t>
+    <x:t>1900091732</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-005</x:t>
@@ -79,7 +79,7 @@
     <x:t>PO-7894</x:t>
   </x:si>
   <x:si>
-    <x:t>1900054909</x:t>
+    <x:t>1900089981</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-006</x:t>
@@ -88,7 +88,7 @@
     <x:t>PO-7895</x:t>
   </x:si>
   <x:si>
-    <x:t>1900028623</x:t>
+    <x:t>1900054759</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-008</x:t>
@@ -97,7 +97,7 @@
     <x:t>PO-7896</x:t>
   </x:si>
   <x:si>
-    <x:t>1900010332</x:t>
+    <x:t>1900094858</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-009</x:t>
@@ -106,7 +106,7 @@
     <x:t>PO-7897</x:t>
   </x:si>
   <x:si>
-    <x:t>1900065727</x:t>
+    <x:t>1900089434</x:t>
   </x:si>
   <x:si>
     <x:t>INV-2025-010</x:t>
@@ -115,7 +115,7 @@
     <x:t>PO-7898</x:t>
   </x:si>
   <x:si>
-    <x:t>1900030682</x:t>
+    <x:t>1900054723</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>